<commit_message>
Finished LinkedIn scraping. So far it searchs, goes down the list of jobs filtering certain aspects like Promoted jobs, Easy Apply, and the company Dice. Once it has gathered all the jobs that meet the criteria, it exports the objects to a xlsx file that can be opened in google sheets.
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,194 +421,109 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Transmission Application Engineer</v>
+        <v>Entry Level Front End Developer</v>
       </c>
       <c r="B2" t="str">
-        <v>Marmon Utility LLC</v>
+        <v>Revature</v>
       </c>
       <c r="C2" t="str">
-        <v>Milford, NH (On-site) Reposted  9 hours ago</v>
+        <v>Brockton, MA On-site 2 hours ago</v>
       </c>
       <c r="D2" t="str">
-        <v>0 applicants</v>
+        <v>11 applicants</v>
       </c>
       <c r="E2" t="str">
-        <v>https://marmon.wd5.myworkdayjobs.com/Marmon_Careers/job/53-Old-Wilton-Road-Milford-NH/Transmission-Application-Engineer_JR0000015994?source=Linkedin</v>
+        <v>https://revature.com/jobs/entry-level-software-engineer-3/?utm_source=linkedin&amp;sourcedBy=BalaLP</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Store Associate, FT</v>
+        <v>Front End Developer - Freelance [Remote]</v>
       </c>
       <c r="B3" t="str">
-        <v>Nike</v>
+        <v>Braintrust</v>
       </c>
       <c r="C3" t="str">
-        <v>Merrimack, NH Reposted  2 hours ago</v>
+        <v>Boston, MA Remote 1 day ago</v>
       </c>
       <c r="D3" t="str">
-        <v>0 applicants</v>
+        <v>112 applicants</v>
       </c>
       <c r="E3" t="str">
-        <v>https://jobs.nike.com/?jobSearch=true&amp;jsOffset=0&amp;jsSort=posting_start_date&amp;jsLanguage=en&amp;error=jobPost</v>
+        <v>https://boards.greenhouse.io/braintrust</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Store Crew (Associates)</v>
+        <v>Front End Engineer</v>
       </c>
       <c r="B4" t="str">
-        <v>Speedway LLC</v>
+        <v>GavinHeath</v>
       </c>
       <c r="C4" t="str">
-        <v>Concord, NH (On-site) Reposted  9 hours ago</v>
+        <v>United States Remote 2 hours ago</v>
       </c>
       <c r="D4" t="str">
-        <v>0 applicants</v>
+        <v>70 applicants</v>
       </c>
       <c r="E4" t="str">
-        <v>https://speedway.wd1.myworkdayjobs.com/Speedway_External_Career_Site/job/Store-1961-Concord-NH/Store-Crew_R-460</v>
+        <v>https://www1.jobdiva.com/portal/?a=k1jdnw97y2ba69mixpqijkgh9633e3075ay54ctusnobplysx8gv35gw2tu44062&amp;jobid=24432843#/jobs/24432843?compid=0&amp;SearchString=&amp;StatesString=&amp;id=24432843&amp;source=linkedin.com</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>PT Center Store Associate Days and Weekend Availability</v>
+        <v>Front-End Developer</v>
       </c>
       <c r="B5" t="str">
-        <v>Hannaford Supermarkets</v>
+        <v>TekVivid, Inc</v>
       </c>
       <c r="C5" t="str">
-        <v>East Hampstead, NH (On-site)  13 hours ago</v>
+        <v>Tewksbury, MA Hybrid 1 hour ago</v>
       </c>
       <c r="D5" t="str">
-        <v>0 applicants</v>
+        <v>6 applicants</v>
       </c>
       <c r="E5" t="str">
-        <v>https://hannaford.careerswithus.com/jobs/?ad=327841_external_USA-NH-East-Hampstead_762023&amp;v=hannafordrms&amp;location=e-hampstead&amp;category=retail-operations&amp;title=pt-center-store-associate-days-and-weekend-availability&amp;utm_source=Linkedin</v>
+        <v>https://tekvivid.oorwin.com/careers/index.html#/job/e26973e6ee8ab9cd8cb3f207d1b90f00d2669eff?source=linkedin_free&amp;postedby=16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Front End Engineer I (Remote)</v>
+        <v>Software Engineer (Front-End)-Minneapolis, MN: 23-01822</v>
       </c>
       <c r="B6" t="str">
-        <v>American Specialty Health</v>
+        <v>Akraya, Inc.</v>
       </c>
       <c r="C6" t="str">
-        <v>United States (Remote) Reposted  15 minutes ago</v>
+        <v>Boston, MA 12 hours ago</v>
       </c>
       <c r="D6" t="str">
-        <v>18 applicants</v>
+        <v>7 applicants</v>
       </c>
       <c r="E6" t="str">
-        <v>https://jobs.jobvite.com/ashcompanies/job/oKZvnfwl</v>
+        <v>https://www2.jobdiva.com/portal/?a=vmjdnwvuqk8ziib1dp1dwwtj5lmlhe03a7vhen21vtdgmiqsu14lwy7xz479eb4w&amp;jobid=20120600#/jobs/20120600?compid=0&amp;SearchString=&amp;StatesString=&amp;id=20120600&amp;source=linkedin.com</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Customer Experience Designer</v>
+        <v>Store Associate, PT - Boston</v>
       </c>
       <c r="B7" t="str">
-        <v>Breezeline</v>
+        <v>Nike</v>
       </c>
       <c r="C7" t="str">
-        <v>Concord, NH (Remote) Reposted  9 hours ago</v>
+        <v>Boston, MA 1 day ago</v>
       </c>
       <c r="D7" t="str">
-        <v>131 applicants</v>
+        <v>2 applicants</v>
       </c>
       <c r="E7" t="str">
-        <v>https://cogeco.wd3.myworkdayjobs.com/en-US/Cogeco_Careers/job/Quincy-MA/Customer-Journey-Manager_JR5976?source=LinkedIn</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Content Management System Back End Developer|| Remote</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Dice</v>
-      </c>
-      <c r="C8" t="str">
-        <v>United States (Remote) Reposted  5 hours ago</v>
-      </c>
-      <c r="D8" t="str">
-        <v>14 applicants</v>
-      </c>
-      <c r="E8" t="str">
-        <v>https://www.dice.com/job-detail/96555968-7e9e-4a9d-b7ac-1f7ad8475d3a?src=32&amp;utm_source=appcast&amp;utm_medium=aggregator&amp;utm_campaign=linkedin-dice-paid&amp;utm_term=Paradigm%20Infotech&amp;utm_content=vp-linkedin-slots_remote_slots&amp;_ccid=1688762495285rg2pue0ci</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Remote Full Stack Software Engineer</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Actalent</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Nashua, NH (Remote)  1 day ago</v>
-      </c>
-      <c r="D9" t="str">
-        <v>38 applicants</v>
-      </c>
-      <c r="E9" t="str">
-        <v>https://careers.actalentservices.com/us/en/job/JP-003885791/Remote-Full-Stack-Software-Engineer?utm_source=Recruitics&amp;utm_medium=equest&amp;s_id=4106&amp;icid=linkedin_recruitics&amp;rx_campaign=Linkedin1&amp;rx_ch=connector&amp;rx_group=125337&amp;rx_job=JP-003885791&amp;rx_medium=post&amp;rx_r=none&amp;rx_source=Linkedin&amp;rx_ts=20230706T184803Z&amp;rx_vp=slots&amp;rx_viewer=e508ea1e1d0611eebb9945f346c91b891b1be452dc824d51ad02afe4fdaf73e4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Remote:- NodeJs/AWS Developer</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Dice</v>
-      </c>
-      <c r="C10" t="str">
-        <v>United States (Remote)  11 hours ago</v>
-      </c>
-      <c r="D10" t="str">
-        <v>50 applicants</v>
-      </c>
-      <c r="E10" t="str">
-        <v>https://www.dice.com/job-detail/0ed92047-54d3-47e8-b8f5-803b48ec9740?src=32&amp;utm_source=appcast&amp;utm_medium=aggregator&amp;utm_campaign=linkedin-dice-paid&amp;utm_term=Corporate%20Biz%20Solutions%20Inc&amp;utm_content=vp-linkedin-slots_most-recent&amp;_ccid=1688762495285rg2pue0ci</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Remote:- NodeJs/AWS Developer</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Dice</v>
-      </c>
-      <c r="C11" t="str">
-        <v>United States (Remote)  11 hours ago</v>
-      </c>
-      <c r="D11" t="str">
-        <v>50 applicants</v>
-      </c>
-      <c r="E11" t="str">
-        <v>https://www.dice.com/job-detail/0ed92047-54d3-47e8-b8f5-803b48ec9740?src=32&amp;utm_source=appcast&amp;utm_medium=aggregator&amp;utm_campaign=linkedin-dice-paid&amp;utm_term=Corporate%20Biz%20Solutions%20Inc&amp;utm_content=vp-linkedin-slots_most-recent&amp;_ccid=1688762495285rg2pue0ci</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Frontend Typescript Developer</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Philotimo-HR</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Greenland, NH (Remote)  7 hours ago</v>
-      </c>
-      <c r="D12" t="str">
-        <v>1 applicant</v>
-      </c>
-      <c r="E12" t="str">
-        <v>https://philotimo.snaphunt.com/job/M34MABCZAR-GL-77?source=linkedin</v>
+        <v>https://jobs.nike.com/job/R-136?source=BY_LinkedIn_OrganicFeed</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>